<commit_message>
updated zoning workbook and zoning function
</commit_message>
<xml_diff>
--- a/Zoning_Workbook.xlsx
+++ b/Zoning_Workbook.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FA6821D-7FCE-4027-B884-692302588A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA709B97-94A4-4696-90A9-7C35F4E585EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{3F8FDE9A-8AA9-43D2-80E0-CEBDCEE92368}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3F8FDE9A-8AA9-43D2-80E0-CEBDCEE92368}"/>
   </bookViews>
   <sheets>
     <sheet name="Frederick County" sheetId="1" r:id="rId1"/>
+    <sheet name="Washington County" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>Zone</t>
   </si>
@@ -153,6 +154,27 @@
   </si>
   <si>
     <t>The purpose of the industrial districts is to provide for the development of varied industrial uses that would supply needed employment opportunities for the county. Industrial development has inherent characteristics that require special attention and protection. Due regard must be given to industrial needs for adequate site locations with concentration on terrain, availability of water and sewer systems, transportation, and compatibility with surrounding development. The Office/Research Industrial District (ORI) is intended to provide for the development of office, research and limited manufacturing uses in high visibility locations along major highways. Development in this district shall be characterized by an absence of nuisances in a clean and aesthetically attractive setting. This district shall permit limited manufacturing, fabrication or assembly operations which would, by nature of the product, or magnitude of production, be compatible with research, professional or business offices. Commercial uses shall be limited to those which are primarily oriented towards servicing those businesses located within the Office/Research Industrial District.</t>
+  </si>
+  <si>
+    <t>Environmental Conservation</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>Washington County Zoning Department</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to prescribe a zoning category for those areas where, because of natural geographic factors and existing land uses, it is considered feasible and desirable to conserve open spaces, water supply sources, woodland areas, wildlife and other natural resources. This district may include extensive steeply sloped areas, stream valleys, water supply sources, and wooded areas adjacent thereto.</t>
+  </si>
+  <si>
+    <t>Preservation</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to prescribe a zoning category for those areas where, because of natural geographic factors and existing land uses, it is considered feasible and desirable to conserve open spaces, water supply sources, woodland areas, wildlife and other natural resources. This district includes the County’s designated Rural Legacy Area, federal lands, state parks, state wildlife management areas, county parks, Edgemont Watershed, and most of the mountaintops and the Potomac River.</t>
   </si>
 </sst>
 </file>
@@ -536,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4386315A-1945-40AB-A178-10267306E6C4}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,4 +880,65 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08200528-FC7B-45B7-B68A-45766BB15ED4}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed language for residential properties in frederick
</commit_message>
<xml_diff>
--- a/Zoning_Workbook.xlsx
+++ b/Zoning_Workbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69109E21-DF89-46E5-9EAE-A9D0DAD717BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2490583-A977-4248-88DF-7ED47E29C3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3F8FDE9A-8AA9-43D2-80E0-CEBDCEE92368}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="112">
   <si>
     <t>Zone</t>
   </si>
@@ -78,9 +78,6 @@
     <t>R-1</t>
   </si>
   <si>
-    <t>The purpose of the residential density districts is to promote healthful and convenient distribution of population with sufficient densities to maintain a high standard of physical design and community service. Residential density districts will conform to the County Comprehensive Plan and will be located within areas identified for residential development. The districts, as a group, are intended to provide for a variety of dwelling types and densities and to offer housing choices at various economic levels. It is further the intent to establish various densities of residential developments in order to efficiently and effectively provide for necessary public services and facilities. The following residential density districts and maximum densities are hereby established.</t>
-  </si>
-  <si>
     <t>R-3</t>
   </si>
   <si>
@@ -370,6 +367,12 @@
   </si>
   <si>
     <t>The purpose of the Education, Research, and Technology District (the "ERT" District) is to provide suitable locations for institutions of higher education, such as two (2) and four (4) year colleges and universities, that will support an environment conducive to higher education and related student life functions and provide compatibility with adjacent land uses. The District will permit all traditional higher education related activities and uses that result from the emerging trends and initiatives toward sharing expertise and facilities between colleges and the business, economic development, technology, and research communities. These uses may include business and technology development services such as incubators and accelerators, applied research, workforce education and training, economic development and research activities that include prototype and limited commodity production and testing, and the provision of structures and facilities within which to conduct such activities.</t>
+  </si>
+  <si>
+    <t>The purpose of the residential density districts is to promote healthful and convenient distribution of population with sufficient densities to maintain a high standard of physical design and community service. Residential density districts will conform to the County Comprehensive Plan and will be located within areas identified for residential development. The districts, as a group, are intended to provide for a variety of dwelling types and densities and to offer housing choices at various economic levels. It is further the intent to establish various densities of residential developments in order to efficiently and effectively provide for necessary public services and facilities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The purpose of the residential density districts is to promote healthful and convenient distribution of population with sufficient densities to maintain a high standard of physical design and community service. Residential density districts will conform to the County Comprehensive Plan and will be located within areas identified for residential development. The districts, as a group, are intended to provide for a variety of dwelling types and densities and to offer housing choices at various economic levels. It is further the intent to establish various densities of residential developments in order to efficiently and effectively provide for necessary public services and facilities. </t>
   </si>
 </sst>
 </file>
@@ -754,7 +757,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +807,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -812,69 +815,69 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -893,86 +896,86 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1109,338 +1112,338 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
       <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
         <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
         <v>61</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
         <v>62</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>64</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
         <v>67</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
         <v>68</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
         <v>70</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
         <v>71</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
         <v>73</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
         <v>76</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
         <v>77</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
         <v>79</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
         <v>80</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
         <v>82</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
         <v>83</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
         <v>85</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
         <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
         <v>88</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
         <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
         <v>91</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
         <v>92</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="s">
         <v>94</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
         <v>95</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
         <v>97</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
         <v>98</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" t="s">
         <v>100</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
         <v>101</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
         <v>103</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
         <v>106</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
         <v>108</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
         <v>109</v>
-      </c>
-      <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added montgomery county to zoning workbook
</commit_message>
<xml_diff>
--- a/Zoning_Workbook.xlsx
+++ b/Zoning_Workbook.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/055abc5dbe1424b0/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E61D822E-6308-4850-AA6C-47D414D70BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{E61D822E-6308-4850-AA6C-47D414D70BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D70978C5-0809-4232-8AE6-F9845BA00846}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3F8FDE9A-8AA9-43D2-80E0-CEBDCEE92368}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{3F8FDE9A-8AA9-43D2-80E0-CEBDCEE92368}"/>
   </bookViews>
   <sheets>
     <sheet name="Frederick County" sheetId="1" r:id="rId1"/>
     <sheet name="Washington County" sheetId="2" r:id="rId2"/>
     <sheet name="Allegany County" sheetId="3" r:id="rId3"/>
+    <sheet name="Montgomery County" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="238">
   <si>
     <t>Zone</t>
   </si>
@@ -512,13 +513,253 @@
   </si>
   <si>
     <t>The purpose of the PD—Planned Development Floating Zone is to encourage the application of innovative and creative land use designs for residential and mixed use developments. The district is intended to allow the unified planning and development of large tracts of land suitable in location, area, and character for the uses and structures proposed</t>
+  </si>
+  <si>
+    <t>Agricultural Reserve</t>
+  </si>
+  <si>
+    <t>Montgomery County Planning and Zoning Department</t>
+  </si>
+  <si>
+    <t>The intent of the AR zone is to promote agriculture as the primary land use in areas of the County designated for agricultural preservation in the general plan, the Functional Master Plan for Preservation of Agriculture and Rural Open Space, and other current or future master plans. The AR zone accomplishes this intent by providing large areas of generally contiguous properties suitable for agricultural and related uses and permitting the transfer of development rights from properties in this zone to properties in designated receiving areas.</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>The intent of the R zone is to preserve rural areas of the County for agriculture and other natural resource development,residential uses of a rural character, extensive recreational facilities, and protection of scenic and environmentally sensitive areas.</t>
+  </si>
+  <si>
+    <t>Rural Cluster</t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>The intent of the RC zone is to provide designated areas of the County for a compatible mixture of agricultural uses and very low-density residential development, to promote agriculture, and to protect scenic and environmentally sensitive areas. The RC zone permits an optional method Cluster Development alternative to provide greater flexibility in achieving a compatible mixture of agricultural and residential uses and to protect scenic and environmentally sensitive areas without jeopardizing farming or other agricultural uses.</t>
+  </si>
+  <si>
+    <t>Rural Neighborhood Cluster</t>
+  </si>
+  <si>
+    <t>RNC</t>
+  </si>
+  <si>
+    <t>The intent of the RNC zone is to preserve open land, environmentally sensitive natural resources, and rural community character through clustering of residential development in the form of small neighborhoods that provide neighborhood identity in an open space setting. A master plan must recommend the RNC zone, and must provide development guidelines and recommendations regarding density, and the location and rationale for preserving the rural open space. It is also the intent of the RNC zone to implement the recommendations of the applicable master plan, such as maintaining broad vistas of open space, preserving agrarian character, or preserving environmentally sensitive natural resources to the maximum extent possible, and to ensure that new development is in harmony with the policies and guidelines of the applicable master plan and is compatible with existing development in adjoining communities.</t>
+  </si>
+  <si>
+    <t>Residential Estate - 2</t>
+  </si>
+  <si>
+    <t>RE-2</t>
+  </si>
+  <si>
+    <t>The intent of the RE-2 zone is to provide designated areas of the County for large-lot residential uses. The predominant use is residential in a detached house.</t>
+  </si>
+  <si>
+    <t>Residential Estate - 2C</t>
+  </si>
+  <si>
+    <t>RE-2C</t>
+  </si>
+  <si>
+    <t>The intent of the RE-2C zone is to provide designated areas of the County for large-lot residential uses. The predominant use is residential in a detached house.</t>
+  </si>
+  <si>
+    <t>Residential Estate - 1</t>
+  </si>
+  <si>
+    <t>RE-1</t>
+  </si>
+  <si>
+    <t>The intent of the RE-1 zone is to provide designated areas of the County for large-lot residential uses. The predominant use is residential in a detached house.</t>
+  </si>
+  <si>
+    <t>Residential - 200</t>
+  </si>
+  <si>
+    <t>R-200</t>
+  </si>
+  <si>
+    <t>The intent of the R-200 zone is to provide designated areas of the County for residential uses with a minimum lot size of 20,000 square feet. The predominant use is residential in a detached house.</t>
+  </si>
+  <si>
+    <t>Residential - 90</t>
+  </si>
+  <si>
+    <t>R-90</t>
+  </si>
+  <si>
+    <t>The intent of the R-90 zone is to provide designated areas of the County for moderate density residential uses. The predominant use is residential in a detached house. A limited number of other building types may be allowed under the optional method of development</t>
+  </si>
+  <si>
+    <t>Residential - 60</t>
+  </si>
+  <si>
+    <t>R-60</t>
+  </si>
+  <si>
+    <t>The intent of the R-60 zone is to provide designated areas of the County for moderate density residential uses. The predominant use is residential in a detached house. A limited number of other building types may be allowed under the optional method of development.</t>
+  </si>
+  <si>
+    <t>Residential - 40</t>
+  </si>
+  <si>
+    <t>R- 40</t>
+  </si>
+  <si>
+    <t>The intent of the R-40 zone is to provide designated areas of the County for moderate density residential uses. The predominant use is residential in a duplex or detached house. A limited number of other building types may be allowed under the optional method of development.</t>
+  </si>
+  <si>
+    <t>Townhouse Low Density</t>
+  </si>
+  <si>
+    <t>TLD</t>
+  </si>
+  <si>
+    <t>The intent of the TLD zone is to provide designated areas of the County for residential purposes at slightly higher densities than the R-90, R-60, and R-40 zones. It is also the intent of the TLD zone to provide a buffer or transition between nonresidential or high-density residential uses and the medium- or low-density Residential zones.</t>
+  </si>
+  <si>
+    <t>Townhouse Medium Density</t>
+  </si>
+  <si>
+    <t>TMD</t>
+  </si>
+  <si>
+    <t>The intent of the TMD zone is to provide designated areas of the County for residential purposes at slightly higher densities than the R-90, R-60, and R-40 zones. It is also the intent of the TMD zone to provide a buffer or transition between nonresidential or high-density residential uses and the medium- or low-density Residential zones.</t>
+  </si>
+  <si>
+    <t>Townhouse High Density</t>
+  </si>
+  <si>
+    <t>THD</t>
+  </si>
+  <si>
+    <t>The intent of the THD zone is to provide designated areas of the County for residential purposes at slightly higher densities than the R-90, R-60, and R-40 zones. It is also the intent of the THD zone to provide a buffer or transition between nonresidential or high-density residential uses and the medium- or low-density Residential zones.</t>
+  </si>
+  <si>
+    <t>Residentual Multi-Unit Low Density</t>
+  </si>
+  <si>
+    <t>R-30</t>
+  </si>
+  <si>
+    <t>The intent of the R-30 zone is to provide designated areas of the County for higher-density, multi-unit residential uses. The predominant use is residential in an apartment building, although detached house, duplex, and townhouse building types are allowed.</t>
+  </si>
+  <si>
+    <t>Residential Multi-Unit Medium Density</t>
+  </si>
+  <si>
+    <t>R-20</t>
+  </si>
+  <si>
+    <t>The intent of the R-20 zone is to provide designated areas of the County for higher-density, multi-unit residential uses. The predominant use is residential in an apartment building, although detached house, duplex, and townhouse building types are allowed.</t>
+  </si>
+  <si>
+    <t>Residential Multi-Unit High Density</t>
+  </si>
+  <si>
+    <t>R-10</t>
+  </si>
+  <si>
+    <t>The intent of the R-10 zone is to provide designated areas of the County for higher-density, multi-unit residential uses. The predominant use is residential in an apartment building, although detached house, duplex, and townhouse building types are allowed.</t>
+  </si>
+  <si>
+    <t>Commercial Residential Neighborhood</t>
+  </si>
+  <si>
+    <t>CRN</t>
+  </si>
+  <si>
+    <t>The CRN zone is intended for pedestrian-scale, neighborhood-serving mixed-use centers and transitional edges. Retail tenant ground floor footprints are limited to preserve community scale.</t>
+  </si>
+  <si>
+    <t>Commercial Residential Town</t>
+  </si>
+  <si>
+    <t>CRT</t>
+  </si>
+  <si>
+    <t>The CRT zone is intended for small downtown, mixed-use, pedestrian-oriented centers and edges of larger, more intense downtowns. Retail tenant ground floor footprints are limited to preserve the town center scale. Transit options may include light rail, Metro, and bus.</t>
+  </si>
+  <si>
+    <t>Commercial Residential</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>The CR zone is intended for larger downtown, mixed-use, and pedestrian-oriented areas in close proximity to transit options such as Metro, light rail, and bus. Retail tenant gross floor area is not restricted.</t>
+  </si>
+  <si>
+    <t>General Retail</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>The GR zone is intended for commercial areas of a general nature, including regional shopping centers and clusters of commercial development. The GR zone provides development opportunities adjacent to the County's most auto-dominated corridors and those areas with few alternative mobility options. The GR zone allows flexibility in building, circulation, and parking lot layout. Retail/Service Establishment gross floor area is not restricted.</t>
+  </si>
+  <si>
+    <t>Neighborhood Retail</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>The NR zone is intended for commercial areas that have a neighborhood orientation and which supply necessities usually requiring frequent purchasing and convenient automobile access. The NR zone addresses development opportunities within primarily residential areas with few alternative mobility options and without a critical mass of density needed for pedestrian-oriented commercial uses. The NR zone allows flexibility in building, circulation, and parking lot layout.</t>
+  </si>
+  <si>
+    <t>Life Sciences Center</t>
+  </si>
+  <si>
+    <t>LSC</t>
+  </si>
+  <si>
+    <t>The LSC zone is intended primarily for research, development, education, and related activities. The primary purpose is to promote research, academic, and clinical facilities that advance the life sciences, health care services, and applied technologies. It is also the purpose of the LSC zone to provide opportunities for the development of uses that support a Life Sciences Center while retaining an environment conducive to high technology research, development, and production. Retail sales and personal services are allowed but are intended for the convenience of employees and residents in the zone.</t>
+  </si>
+  <si>
+    <t>Employment Office</t>
+  </si>
+  <si>
+    <t>EOF</t>
+  </si>
+  <si>
+    <t>The EOF zone is intended for office and employment activity combined with limited residential and neighborhood commercial uses. The EOF allows flexibility in building, circulation, and parking lot layout.</t>
+  </si>
+  <si>
+    <t>Light Industrial</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>The IL zone is intended to provide land for industrial activities where major transportation links are not typically necessary and noise, dust, vibration, glare, odors, and other adverse environmental impacts are usually minimal. The IL zone is appropriate as a transitional Industrial zone between a Residentially zoned area and land classified in the IM and IH zones.</t>
+  </si>
+  <si>
+    <t>Moderate Industrial</t>
+  </si>
+  <si>
+    <t>The IM zone is intended to provide land for industrial activities where major transportation links are not typically necessary and noise, dust, vibration, glare, odors, and other adverse environmental impacts are usually minimal.</t>
+  </si>
+  <si>
+    <t>Heavy Industrial</t>
+  </si>
+  <si>
+    <t>IH</t>
+  </si>
+  <si>
+    <t>The IH zone is intended to provide land for industrial activities that usually need major transportation links to highways or rail and may create significant noise, dust, vibration, glare, odors, and other adverse environmental impacts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -530,6 +771,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Corbel"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -553,12 +800,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,6 +822,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1594,7 +1846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756DDD1D-AC87-411F-A32F-D80E159BFE9F}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1831,4 +2085,417 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35581AC-AE9A-4889-8D41-80F11D0C61A0}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B23" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" t="s">
+        <v>159</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B26" t="s">
+        <v>231</v>
+      </c>
+      <c r="C26" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>233</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>235</v>
+      </c>
+      <c r="B28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed value error and added unzoned to Garrett County
</commit_message>
<xml_diff>
--- a/Zoning_Workbook.xlsx
+++ b/Zoning_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/055abc5dbe1424b0/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{B403492E-D524-470A-817F-100DC0F063C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75623CF6-BCD9-426E-ACC5-108559479D62}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{B403492E-D524-470A-817F-100DC0F063C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A6781DC-51DA-43C0-B3C4-168F27F69CAE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{3F8FDE9A-8AA9-43D2-80E0-CEBDCEE92368}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="263">
   <si>
     <t>Zone</t>
   </si>
@@ -826,6 +826,9 @@
   </si>
   <si>
     <t>The purpose of the Commercial Resort 2 district is to provide for commercial recreation uses and supporting commercial activities. To promote resort-type light commercial uses and family recreation, while avoiding heavy highway commercial development. The Commercial Resort 1 district provides opportunities for visitor-oriented commercial development, but not major residential development. The Commercial Resort 2 district emphasizes land-based family-oriented development, while allowing for residential development at an average density of 1 unit per acre.</t>
+  </si>
+  <si>
+    <t>Unzoned</t>
   </si>
 </sst>
 </file>
@@ -901,6 +904,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2577,9 +2584,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B876379D-006F-4A43-9039-6951AB347211}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2729,6 +2738,11 @@
         <v>261</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>262</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>